<commit_message>
edit summary timesheet report
</commit_message>
<xml_diff>
--- a/server/storage/private/report/Playtorium_Summary_Timesheet.xlsx
+++ b/server/storage/private/report/Playtorium_Summary_Timesheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmark_s/Documents/playtorium/emp-management/server/storage/private/report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmark_s/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,12 +523,6 @@
       <color theme="9" tint="-0.499984740745262"/>
       <name val="Angsana New"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -981,11 +975,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R132"/>
+  <dimension ref="B2:R186"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -993,8 +987,8 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="16" width="6.83203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="6.5" customWidth="1"/>
+    <col min="6" max="16" width="6.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3053,65 +3047,773 @@
       <c r="O127"/>
       <c r="P127"/>
     </row>
-    <row r="129" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D129" s="7"/>
-      <c r="E129" s="7"/>
-      <c r="F129" s="8"/>
-      <c r="G129" s="8"/>
-      <c r="H129" s="8"/>
-      <c r="I129" s="8"/>
-      <c r="J129" s="8"/>
-      <c r="K129" s="8"/>
-      <c r="L129" s="8"/>
-      <c r="M129" s="8"/>
-      <c r="N129" s="8"/>
-      <c r="O129" s="8"/>
-      <c r="P129" s="8"/>
-    </row>
-    <row r="130" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D130" s="7"/>
-      <c r="E130" s="7"/>
-      <c r="F130" s="8"/>
-      <c r="G130" s="8"/>
-      <c r="H130" s="8"/>
-      <c r="I130" s="8"/>
-      <c r="J130" s="8"/>
-      <c r="K130" s="8"/>
-      <c r="L130" s="8"/>
-      <c r="M130" s="8"/>
-      <c r="N130" s="8"/>
-      <c r="O130" s="8"/>
-      <c r="P130" s="8"/>
-    </row>
-    <row r="131" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D131" s="7"/>
-      <c r="E131" s="7"/>
-      <c r="F131" s="8"/>
-      <c r="G131" s="8"/>
-      <c r="H131" s="8"/>
-      <c r="I131" s="8"/>
-      <c r="J131" s="8"/>
-      <c r="K131" s="8"/>
-      <c r="L131" s="8"/>
-      <c r="M131" s="8"/>
-      <c r="N131" s="8"/>
-      <c r="O131" s="8"/>
-      <c r="P131" s="8"/>
-    </row>
-    <row r="132" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D132" s="7"/>
-      <c r="E132" s="7"/>
-      <c r="F132" s="8"/>
-      <c r="G132" s="8"/>
-      <c r="H132" s="8"/>
-      <c r="I132" s="8"/>
-      <c r="J132" s="8"/>
-      <c r="K132" s="8"/>
-      <c r="L132" s="8"/>
-      <c r="M132" s="8"/>
-      <c r="N132" s="8"/>
-      <c r="P132" s="8"/>
+    <row r="128" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="F128"/>
+      <c r="G128"/>
+      <c r="H128"/>
+      <c r="I128"/>
+      <c r="J128"/>
+      <c r="K128"/>
+      <c r="L128"/>
+      <c r="M128"/>
+      <c r="N128"/>
+      <c r="O128"/>
+      <c r="P128"/>
+    </row>
+    <row r="129" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F129"/>
+      <c r="G129"/>
+      <c r="H129"/>
+      <c r="I129"/>
+      <c r="J129"/>
+      <c r="K129"/>
+      <c r="L129"/>
+      <c r="M129"/>
+      <c r="N129"/>
+      <c r="O129"/>
+      <c r="P129"/>
+    </row>
+    <row r="130" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F130"/>
+      <c r="G130"/>
+      <c r="H130"/>
+      <c r="I130"/>
+      <c r="J130"/>
+      <c r="K130"/>
+      <c r="L130"/>
+      <c r="M130"/>
+      <c r="N130"/>
+      <c r="O130"/>
+      <c r="P130"/>
+    </row>
+    <row r="131" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F131"/>
+      <c r="G131"/>
+      <c r="H131"/>
+      <c r="I131"/>
+      <c r="J131"/>
+      <c r="K131"/>
+      <c r="L131"/>
+      <c r="M131"/>
+      <c r="N131"/>
+      <c r="O131"/>
+      <c r="P131"/>
+    </row>
+    <row r="132" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F132"/>
+      <c r="G132"/>
+      <c r="H132"/>
+      <c r="I132"/>
+      <c r="J132"/>
+      <c r="K132"/>
+      <c r="L132"/>
+      <c r="M132"/>
+      <c r="N132"/>
+      <c r="O132"/>
+      <c r="P132"/>
       <c r="R132" s="8"/>
+    </row>
+    <row r="133" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F133"/>
+      <c r="G133"/>
+      <c r="H133"/>
+      <c r="I133"/>
+      <c r="J133"/>
+      <c r="K133"/>
+      <c r="L133"/>
+      <c r="M133"/>
+      <c r="N133"/>
+      <c r="O133"/>
+      <c r="P133"/>
+    </row>
+    <row r="134" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F134"/>
+      <c r="G134"/>
+      <c r="H134"/>
+      <c r="I134"/>
+      <c r="J134"/>
+      <c r="K134"/>
+      <c r="L134"/>
+      <c r="M134"/>
+      <c r="N134"/>
+      <c r="O134"/>
+      <c r="P134"/>
+    </row>
+    <row r="135" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F135"/>
+      <c r="G135"/>
+      <c r="H135"/>
+      <c r="I135"/>
+      <c r="J135"/>
+      <c r="K135"/>
+      <c r="L135"/>
+      <c r="M135"/>
+      <c r="N135"/>
+      <c r="O135"/>
+      <c r="P135"/>
+    </row>
+    <row r="136" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F136"/>
+      <c r="G136"/>
+      <c r="H136"/>
+      <c r="I136"/>
+      <c r="J136"/>
+      <c r="K136"/>
+      <c r="L136"/>
+      <c r="M136"/>
+      <c r="N136"/>
+      <c r="O136"/>
+      <c r="P136"/>
+    </row>
+    <row r="137" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F137"/>
+      <c r="G137"/>
+      <c r="H137"/>
+      <c r="I137"/>
+      <c r="J137"/>
+      <c r="K137"/>
+      <c r="L137"/>
+      <c r="M137"/>
+      <c r="N137"/>
+      <c r="O137"/>
+      <c r="P137"/>
+    </row>
+    <row r="138" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F138"/>
+      <c r="G138"/>
+      <c r="H138"/>
+      <c r="I138"/>
+      <c r="J138"/>
+      <c r="K138"/>
+      <c r="L138"/>
+      <c r="M138"/>
+      <c r="N138"/>
+      <c r="O138"/>
+      <c r="P138"/>
+    </row>
+    <row r="139" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F139"/>
+      <c r="G139"/>
+      <c r="H139"/>
+      <c r="I139"/>
+      <c r="J139"/>
+      <c r="K139"/>
+      <c r="L139"/>
+      <c r="M139"/>
+      <c r="N139"/>
+      <c r="O139"/>
+      <c r="P139"/>
+    </row>
+    <row r="140" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F140"/>
+      <c r="G140"/>
+      <c r="H140"/>
+      <c r="I140"/>
+      <c r="J140"/>
+      <c r="K140"/>
+      <c r="L140"/>
+      <c r="M140"/>
+      <c r="N140"/>
+      <c r="O140"/>
+      <c r="P140"/>
+    </row>
+    <row r="141" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F141"/>
+      <c r="G141"/>
+      <c r="H141"/>
+      <c r="I141"/>
+      <c r="J141"/>
+      <c r="K141"/>
+      <c r="L141"/>
+      <c r="M141"/>
+      <c r="N141"/>
+      <c r="O141"/>
+      <c r="P141"/>
+    </row>
+    <row r="142" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F142"/>
+      <c r="G142"/>
+      <c r="H142"/>
+      <c r="I142"/>
+      <c r="J142"/>
+      <c r="K142"/>
+      <c r="L142"/>
+      <c r="M142"/>
+      <c r="N142"/>
+      <c r="O142"/>
+      <c r="P142"/>
+    </row>
+    <row r="143" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F143"/>
+      <c r="G143"/>
+      <c r="H143"/>
+      <c r="I143"/>
+      <c r="J143"/>
+      <c r="K143"/>
+      <c r="L143"/>
+      <c r="M143"/>
+      <c r="N143"/>
+      <c r="O143"/>
+      <c r="P143"/>
+    </row>
+    <row r="144" spans="6:18" x14ac:dyDescent="0.2">
+      <c r="F144"/>
+      <c r="G144"/>
+      <c r="H144"/>
+      <c r="I144"/>
+      <c r="J144"/>
+      <c r="K144"/>
+      <c r="L144"/>
+      <c r="M144"/>
+      <c r="N144"/>
+      <c r="O144"/>
+      <c r="P144"/>
+    </row>
+    <row r="145" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F145"/>
+      <c r="G145"/>
+      <c r="H145"/>
+      <c r="I145"/>
+      <c r="J145"/>
+      <c r="K145"/>
+      <c r="L145"/>
+      <c r="M145"/>
+      <c r="N145"/>
+      <c r="O145"/>
+      <c r="P145"/>
+    </row>
+    <row r="146" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F146"/>
+      <c r="G146"/>
+      <c r="H146"/>
+      <c r="I146"/>
+      <c r="J146"/>
+      <c r="K146"/>
+      <c r="L146"/>
+      <c r="M146"/>
+      <c r="N146"/>
+      <c r="O146"/>
+      <c r="P146"/>
+    </row>
+    <row r="147" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F147"/>
+      <c r="G147"/>
+      <c r="H147"/>
+      <c r="I147"/>
+      <c r="J147"/>
+      <c r="K147"/>
+      <c r="L147"/>
+      <c r="M147"/>
+      <c r="N147"/>
+      <c r="O147"/>
+      <c r="P147"/>
+    </row>
+    <row r="148" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F148"/>
+      <c r="G148"/>
+      <c r="H148"/>
+      <c r="I148"/>
+      <c r="J148"/>
+      <c r="K148"/>
+      <c r="L148"/>
+      <c r="M148"/>
+      <c r="N148"/>
+      <c r="O148"/>
+      <c r="P148"/>
+    </row>
+    <row r="149" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F149"/>
+      <c r="G149"/>
+      <c r="H149"/>
+      <c r="I149"/>
+      <c r="J149"/>
+      <c r="K149"/>
+      <c r="L149"/>
+      <c r="M149"/>
+      <c r="N149"/>
+      <c r="O149"/>
+      <c r="P149"/>
+    </row>
+    <row r="150" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F150"/>
+      <c r="G150"/>
+      <c r="H150"/>
+      <c r="I150"/>
+      <c r="J150"/>
+      <c r="K150"/>
+      <c r="L150"/>
+      <c r="M150"/>
+      <c r="N150"/>
+      <c r="O150"/>
+      <c r="P150"/>
+    </row>
+    <row r="151" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F151"/>
+      <c r="G151"/>
+      <c r="H151"/>
+      <c r="I151"/>
+      <c r="J151"/>
+      <c r="K151"/>
+      <c r="L151"/>
+      <c r="M151"/>
+      <c r="N151"/>
+      <c r="O151"/>
+      <c r="P151"/>
+    </row>
+    <row r="152" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F152"/>
+      <c r="G152"/>
+      <c r="H152"/>
+      <c r="I152"/>
+      <c r="J152"/>
+      <c r="K152"/>
+      <c r="L152"/>
+      <c r="M152"/>
+      <c r="N152"/>
+      <c r="O152"/>
+      <c r="P152"/>
+    </row>
+    <row r="153" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F153"/>
+      <c r="G153"/>
+      <c r="H153"/>
+      <c r="I153"/>
+      <c r="J153"/>
+      <c r="K153"/>
+      <c r="L153"/>
+      <c r="M153"/>
+      <c r="N153"/>
+      <c r="O153"/>
+      <c r="P153"/>
+    </row>
+    <row r="154" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F154"/>
+      <c r="G154"/>
+      <c r="H154"/>
+      <c r="I154"/>
+      <c r="J154"/>
+      <c r="K154"/>
+      <c r="L154"/>
+      <c r="M154"/>
+      <c r="N154"/>
+      <c r="O154"/>
+      <c r="P154"/>
+    </row>
+    <row r="155" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F155"/>
+      <c r="G155"/>
+      <c r="H155"/>
+      <c r="I155"/>
+      <c r="J155"/>
+      <c r="K155"/>
+      <c r="L155"/>
+      <c r="M155"/>
+      <c r="N155"/>
+      <c r="O155"/>
+      <c r="P155"/>
+    </row>
+    <row r="156" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F156"/>
+      <c r="G156"/>
+      <c r="H156"/>
+      <c r="I156"/>
+      <c r="J156"/>
+      <c r="K156"/>
+      <c r="L156"/>
+      <c r="M156"/>
+      <c r="N156"/>
+      <c r="O156"/>
+      <c r="P156"/>
+    </row>
+    <row r="157" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F157"/>
+      <c r="G157"/>
+      <c r="H157"/>
+      <c r="I157"/>
+      <c r="J157"/>
+      <c r="K157"/>
+      <c r="L157"/>
+      <c r="M157"/>
+      <c r="N157"/>
+      <c r="O157"/>
+      <c r="P157"/>
+    </row>
+    <row r="158" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F158"/>
+      <c r="G158"/>
+      <c r="H158"/>
+      <c r="I158"/>
+      <c r="J158"/>
+      <c r="K158"/>
+      <c r="L158"/>
+      <c r="M158"/>
+      <c r="N158"/>
+      <c r="O158"/>
+      <c r="P158"/>
+    </row>
+    <row r="159" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F159"/>
+      <c r="G159"/>
+      <c r="H159"/>
+      <c r="I159"/>
+      <c r="J159"/>
+      <c r="K159"/>
+      <c r="L159"/>
+      <c r="M159"/>
+      <c r="N159"/>
+      <c r="O159"/>
+      <c r="P159"/>
+    </row>
+    <row r="160" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F160"/>
+      <c r="G160"/>
+      <c r="H160"/>
+      <c r="I160"/>
+      <c r="J160"/>
+      <c r="K160"/>
+      <c r="L160"/>
+      <c r="M160"/>
+      <c r="N160"/>
+      <c r="O160"/>
+      <c r="P160"/>
+    </row>
+    <row r="161" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F161"/>
+      <c r="G161"/>
+      <c r="H161"/>
+      <c r="I161"/>
+      <c r="J161"/>
+      <c r="K161"/>
+      <c r="L161"/>
+      <c r="M161"/>
+      <c r="N161"/>
+      <c r="O161"/>
+      <c r="P161"/>
+    </row>
+    <row r="162" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F162"/>
+      <c r="G162"/>
+      <c r="H162"/>
+      <c r="I162"/>
+      <c r="J162"/>
+      <c r="K162"/>
+      <c r="L162"/>
+      <c r="M162"/>
+      <c r="N162"/>
+      <c r="O162"/>
+      <c r="P162"/>
+    </row>
+    <row r="163" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F163"/>
+      <c r="G163"/>
+      <c r="H163"/>
+      <c r="I163"/>
+      <c r="J163"/>
+      <c r="K163"/>
+      <c r="L163"/>
+      <c r="M163"/>
+      <c r="N163"/>
+      <c r="O163"/>
+      <c r="P163"/>
+    </row>
+    <row r="164" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F164"/>
+      <c r="G164"/>
+      <c r="H164"/>
+      <c r="I164"/>
+      <c r="J164"/>
+      <c r="K164"/>
+      <c r="L164"/>
+      <c r="M164"/>
+      <c r="N164"/>
+      <c r="O164"/>
+      <c r="P164"/>
+    </row>
+    <row r="165" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F165"/>
+      <c r="G165"/>
+      <c r="H165"/>
+      <c r="I165"/>
+      <c r="J165"/>
+      <c r="K165"/>
+      <c r="L165"/>
+      <c r="M165"/>
+      <c r="N165"/>
+      <c r="O165"/>
+      <c r="P165"/>
+    </row>
+    <row r="166" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F166"/>
+      <c r="G166"/>
+      <c r="H166"/>
+      <c r="I166"/>
+      <c r="J166"/>
+      <c r="K166"/>
+      <c r="L166"/>
+      <c r="M166"/>
+      <c r="N166"/>
+      <c r="O166"/>
+      <c r="P166"/>
+    </row>
+    <row r="167" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F167"/>
+      <c r="G167"/>
+      <c r="H167"/>
+      <c r="I167"/>
+      <c r="J167"/>
+      <c r="K167"/>
+      <c r="L167"/>
+      <c r="M167"/>
+      <c r="N167"/>
+      <c r="O167"/>
+      <c r="P167"/>
+    </row>
+    <row r="168" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F168"/>
+      <c r="G168"/>
+      <c r="H168"/>
+      <c r="I168"/>
+      <c r="J168"/>
+      <c r="K168"/>
+      <c r="L168"/>
+      <c r="M168"/>
+      <c r="N168"/>
+      <c r="O168"/>
+      <c r="P168"/>
+    </row>
+    <row r="169" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F169"/>
+      <c r="G169"/>
+      <c r="H169"/>
+      <c r="I169"/>
+      <c r="J169"/>
+      <c r="K169"/>
+      <c r="L169"/>
+      <c r="M169"/>
+      <c r="N169"/>
+      <c r="O169"/>
+      <c r="P169"/>
+    </row>
+    <row r="170" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F170"/>
+      <c r="G170"/>
+      <c r="H170"/>
+      <c r="I170"/>
+      <c r="J170"/>
+      <c r="K170"/>
+      <c r="L170"/>
+      <c r="M170"/>
+      <c r="N170"/>
+      <c r="O170"/>
+      <c r="P170"/>
+    </row>
+    <row r="171" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F171"/>
+      <c r="G171"/>
+      <c r="H171"/>
+      <c r="I171"/>
+      <c r="J171"/>
+      <c r="K171"/>
+      <c r="L171"/>
+      <c r="M171"/>
+      <c r="N171"/>
+      <c r="O171"/>
+      <c r="P171"/>
+    </row>
+    <row r="172" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F172"/>
+      <c r="G172"/>
+      <c r="H172"/>
+      <c r="I172"/>
+      <c r="J172"/>
+      <c r="K172"/>
+      <c r="L172"/>
+      <c r="M172"/>
+      <c r="N172"/>
+      <c r="O172"/>
+      <c r="P172"/>
+    </row>
+    <row r="173" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F173"/>
+      <c r="G173"/>
+      <c r="H173"/>
+      <c r="I173"/>
+      <c r="J173"/>
+      <c r="K173"/>
+      <c r="L173"/>
+      <c r="M173"/>
+      <c r="N173"/>
+      <c r="O173"/>
+      <c r="P173"/>
+    </row>
+    <row r="174" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F174"/>
+      <c r="G174"/>
+      <c r="H174"/>
+      <c r="I174"/>
+      <c r="J174"/>
+      <c r="K174"/>
+      <c r="L174"/>
+      <c r="M174"/>
+      <c r="N174"/>
+      <c r="O174"/>
+      <c r="P174"/>
+    </row>
+    <row r="175" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F175"/>
+      <c r="G175"/>
+      <c r="H175"/>
+      <c r="I175"/>
+      <c r="J175"/>
+      <c r="K175"/>
+      <c r="L175"/>
+      <c r="M175"/>
+      <c r="N175"/>
+      <c r="O175"/>
+      <c r="P175"/>
+    </row>
+    <row r="176" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F176"/>
+      <c r="G176"/>
+      <c r="H176"/>
+      <c r="I176"/>
+      <c r="J176"/>
+      <c r="K176"/>
+      <c r="L176"/>
+      <c r="M176"/>
+      <c r="N176"/>
+      <c r="O176"/>
+      <c r="P176"/>
+    </row>
+    <row r="177" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F177"/>
+      <c r="G177"/>
+      <c r="H177"/>
+      <c r="I177"/>
+      <c r="J177"/>
+      <c r="K177"/>
+      <c r="L177"/>
+      <c r="M177"/>
+      <c r="N177"/>
+      <c r="O177"/>
+      <c r="P177"/>
+    </row>
+    <row r="178" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F178"/>
+      <c r="G178"/>
+      <c r="H178"/>
+      <c r="I178"/>
+      <c r="J178"/>
+      <c r="K178"/>
+      <c r="L178"/>
+      <c r="M178"/>
+      <c r="N178"/>
+      <c r="O178"/>
+      <c r="P178"/>
+    </row>
+    <row r="179" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F179"/>
+      <c r="G179"/>
+      <c r="H179"/>
+      <c r="I179"/>
+      <c r="J179"/>
+      <c r="K179"/>
+      <c r="L179"/>
+      <c r="M179"/>
+      <c r="N179"/>
+      <c r="O179"/>
+      <c r="P179"/>
+    </row>
+    <row r="180" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F180"/>
+      <c r="G180"/>
+      <c r="H180"/>
+      <c r="I180"/>
+      <c r="J180"/>
+      <c r="K180"/>
+      <c r="L180"/>
+      <c r="M180"/>
+      <c r="N180"/>
+      <c r="O180"/>
+      <c r="P180"/>
+    </row>
+    <row r="181" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F181"/>
+      <c r="G181"/>
+      <c r="H181"/>
+      <c r="I181"/>
+      <c r="J181"/>
+      <c r="K181"/>
+      <c r="L181"/>
+      <c r="M181"/>
+      <c r="N181"/>
+      <c r="O181"/>
+      <c r="P181"/>
+    </row>
+    <row r="182" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F182"/>
+      <c r="G182"/>
+      <c r="H182"/>
+      <c r="I182"/>
+      <c r="J182"/>
+      <c r="K182"/>
+      <c r="L182"/>
+      <c r="M182"/>
+      <c r="N182"/>
+      <c r="O182"/>
+      <c r="P182"/>
+    </row>
+    <row r="183" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F183"/>
+      <c r="G183"/>
+      <c r="H183"/>
+      <c r="I183"/>
+      <c r="J183"/>
+      <c r="K183"/>
+      <c r="L183"/>
+      <c r="M183"/>
+      <c r="N183"/>
+      <c r="O183"/>
+      <c r="P183"/>
+    </row>
+    <row r="184" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F184"/>
+      <c r="G184"/>
+      <c r="H184"/>
+      <c r="I184"/>
+      <c r="J184"/>
+      <c r="K184"/>
+      <c r="L184"/>
+      <c r="M184"/>
+      <c r="N184"/>
+      <c r="O184"/>
+      <c r="P184"/>
+    </row>
+    <row r="185" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F185"/>
+      <c r="G185"/>
+      <c r="H185"/>
+      <c r="I185"/>
+      <c r="J185"/>
+      <c r="K185"/>
+      <c r="L185"/>
+      <c r="M185"/>
+      <c r="N185"/>
+      <c r="O185"/>
+      <c r="P185"/>
+    </row>
+    <row r="186" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F186"/>
+      <c r="G186"/>
+      <c r="H186"/>
+      <c r="I186"/>
+      <c r="J186"/>
+      <c r="K186"/>
+      <c r="L186"/>
+      <c r="M186"/>
+      <c r="N186"/>
+      <c r="O186"/>
+      <c r="P186"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:P125">
@@ -3130,9 +3832,8 @@
   <mergeCells count="1">
     <mergeCell ref="E2:P2"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>